<commit_message>
Sistemato check sbagliato secondo ciclo while
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_input/Scheda_Macchine_Taglio.xlsx
+++ b/PS-VRP/Dati_input/Scheda_Macchine_Taglio.xlsx
@@ -459,19 +459,19 @@
         <v>28</v>
       </c>
       <c r="B2" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="8">
         <v>156</v>
       </c>
       <c r="D2" s="9">
-        <v>61</v>
+        <v>120</v>
       </c>
       <c r="E2" t="s" s="10">
         <v>29</v>
       </c>
       <c r="F2" s="11">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G2" s="12">
         <v>70</v>
@@ -504,7 +504,7 @@
         <v>500</v>
       </c>
       <c r="T2" s="25">
-        <v>45812</v>
+        <v>45846</v>
       </c>
       <c r="U2" s="26">
         <v>.2916666666666673352208</v>
@@ -542,13 +542,13 @@
         <v>168</v>
       </c>
       <c r="D3" s="9">
-        <v>71</v>
+        <v>120</v>
       </c>
       <c r="E3" t="s" s="10">
         <v>29</v>
       </c>
       <c r="F3" s="11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G3" s="12">
         <v>76</v>
@@ -584,7 +584,7 @@
         <v>50</v>
       </c>
       <c r="T3" s="25">
-        <v>45813</v>
+        <v>45846</v>
       </c>
       <c r="U3" s="26">
         <v>.2916666666666673352208</v>
@@ -616,19 +616,19 @@
         <v>35</v>
       </c>
       <c r="B4" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="8">
         <v>101</v>
       </c>
       <c r="D4" s="9">
-        <v>64</v>
+        <v>120</v>
       </c>
       <c r="E4" t="s" s="10">
         <v>29</v>
       </c>
       <c r="F4" s="11">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G4" s="12">
         <v>70</v>
@@ -664,10 +664,10 @@
         <v>50</v>
       </c>
       <c r="T4" s="25">
-        <v>45813</v>
+        <v>45846</v>
       </c>
       <c r="U4" s="26">
-        <v>.5000000000000011460928</v>
+        <v>.2916666666666673352208</v>
       </c>
       <c r="V4" s="27">
         <v>15</v>
@@ -702,13 +702,13 @@
         <v>100</v>
       </c>
       <c r="D5" s="9">
-        <v>71</v>
+        <v>120</v>
       </c>
       <c r="E5" t="s" s="10">
         <v>29</v>
       </c>
       <c r="F5" s="11">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G5" s="12">
         <v>76</v>
@@ -744,10 +744,10 @@
         <v>50</v>
       </c>
       <c r="T5" s="25">
-        <v>45812</v>
+        <v>45846</v>
       </c>
       <c r="U5" s="26">
-        <v>.5000000000000011460928</v>
+        <v>.2916666666666673352208</v>
       </c>
       <c r="V5" s="27">
         <v>15</v>
@@ -782,13 +782,13 @@
         <v>123</v>
       </c>
       <c r="D6" s="9">
-        <v>55</v>
+        <v>120</v>
       </c>
       <c r="E6" t="s" s="10">
         <v>29</v>
       </c>
       <c r="F6" s="11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G6" s="12">
         <v>70</v>
@@ -821,7 +821,7 @@
         <v>500</v>
       </c>
       <c r="T6" s="25">
-        <v>45813</v>
+        <v>45846</v>
       </c>
       <c r="U6" s="26">
         <v>.2916666666666673352208</v>
@@ -853,13 +853,13 @@
         <v>41</v>
       </c>
       <c r="B7" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="8">
         <v>103</v>
       </c>
       <c r="D7" s="9">
-        <v>49</v>
+        <v>120</v>
       </c>
       <c r="E7" t="s" s="10">
         <v>29</v>
@@ -898,7 +898,7 @@
         <v>420</v>
       </c>
       <c r="T7" s="25">
-        <v>45812</v>
+        <v>45846</v>
       </c>
       <c r="U7" s="26">
         <v>.2916666666666673352208</v>
@@ -936,16 +936,13 @@
         <v>118</v>
       </c>
       <c r="D8" s="9">
-        <v>61</v>
+        <v>120</v>
       </c>
       <c r="E8" t="s" s="10">
         <v>29</v>
       </c>
       <c r="F8" s="11">
-        <v>3</v>
-      </c>
-      <c r="G8" s="12">
-        <v>76</v>
+        <v>1</v>
       </c>
       <c r="H8" s="13">
         <v>400</v>
@@ -978,7 +975,7 @@
         <v>50</v>
       </c>
       <c r="T8" s="25">
-        <v>45813</v>
+        <v>45846</v>
       </c>
       <c r="U8" s="26">
         <v>.2916666666666673352208</v>
@@ -1016,16 +1013,16 @@
         <v>176</v>
       </c>
       <c r="D9" s="9">
-        <v>69</v>
+        <v>120</v>
       </c>
       <c r="E9" t="s" s="10">
         <v>29</v>
       </c>
       <c r="F9" s="11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G9" s="12">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="H9" s="13">
         <v>0</v>
@@ -1055,7 +1052,7 @@
         <v>600</v>
       </c>
       <c r="T9" s="25">
-        <v>45814</v>
+        <v>45846</v>
       </c>
       <c r="U9" s="26">
         <v>.2916666666666673352208</v>
@@ -1087,13 +1084,13 @@
         <v>47</v>
       </c>
       <c r="B10" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="8">
         <v>169</v>
       </c>
       <c r="D10" s="9">
-        <v>71</v>
+        <v>120</v>
       </c>
       <c r="E10" t="s" s="10">
         <v>29</v>
@@ -1135,7 +1132,7 @@
         <v>18</v>
       </c>
       <c r="T10" s="25">
-        <v>45813</v>
+        <v>45846</v>
       </c>
       <c r="U10" s="26">
         <v>.2916666666666673352208</v>
@@ -1173,13 +1170,13 @@
         <v>181</v>
       </c>
       <c r="D11" s="9">
-        <v>54</v>
+        <v>120</v>
       </c>
       <c r="E11" t="s" s="10">
         <v>29</v>
       </c>
       <c r="F11" s="11">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G11" s="12">
         <v>70</v>
@@ -1215,10 +1212,10 @@
         <v>40</v>
       </c>
       <c r="T11" s="25">
-        <v>45812</v>
+        <v>45846</v>
       </c>
       <c r="U11" s="26">
-        <v>.5000000000000011460928</v>
+        <v>.2916666666666673352208</v>
       </c>
       <c r="V11" s="27">
         <v>10</v>
@@ -1253,16 +1250,16 @@
         <v>118</v>
       </c>
       <c r="D12" s="9">
-        <v>70</v>
+        <v>120</v>
       </c>
       <c r="E12" t="s" s="10">
         <v>29</v>
       </c>
       <c r="F12" s="11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G12" s="12">
-        <v>70</v>
+        <v>152</v>
       </c>
       <c r="H12" s="13">
         <v>0</v>
@@ -1292,7 +1289,7 @@
         <v>600</v>
       </c>
       <c r="T12" s="25">
-        <v>45812</v>
+        <v>45846</v>
       </c>
       <c r="U12" s="26">
         <v>.2916666666666673352208</v>
@@ -1330,13 +1327,16 @@
         <v>192</v>
       </c>
       <c r="D13" s="9">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="E13" t="s" s="10">
         <v>29</v>
       </c>
       <c r="F13" s="11">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="G13" s="12">
+        <v>76</v>
       </c>
       <c r="H13" s="13">
         <v>400</v>
@@ -1369,10 +1369,10 @@
         <v>50</v>
       </c>
       <c r="T13" s="25">
-        <v>45813</v>
+        <v>45846</v>
       </c>
       <c r="U13" s="26">
-        <v>.5000000000000011460928</v>
+        <v>.2916666666666673352208</v>
       </c>
       <c r="V13" s="27">
         <v>15</v>
@@ -1401,13 +1401,13 @@
         <v>55</v>
       </c>
       <c r="B14" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" s="8">
         <v>104</v>
       </c>
       <c r="D14" s="9">
-        <v>63</v>
+        <v>120</v>
       </c>
       <c r="E14" t="s" s="10">
         <v>56</v>
@@ -1437,7 +1437,7 @@
         <v>640</v>
       </c>
       <c r="T14" s="25">
-        <v>45814</v>
+        <v>45846</v>
       </c>
       <c r="U14" s="26">
         <v>.2916666666666673352208</v>
@@ -1448,13 +1448,13 @@
         <v>59</v>
       </c>
       <c r="B15" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" s="8">
         <v>169</v>
       </c>
       <c r="D15" s="9">
-        <v>63</v>
+        <v>120</v>
       </c>
       <c r="E15" t="s" s="10">
         <v>56</v>
@@ -1484,7 +1484,7 @@
         <v>1000</v>
       </c>
       <c r="T15" s="25">
-        <v>45813</v>
+        <v>45846</v>
       </c>
       <c r="U15" s="26">
         <v>.2916666666666673352208</v>
@@ -1495,13 +1495,13 @@
         <v>61</v>
       </c>
       <c r="B16" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" s="8">
         <v>195</v>
       </c>
       <c r="D16" s="9">
-        <v>63</v>
+        <v>120</v>
       </c>
       <c r="E16" t="s" s="10">
         <v>56</v>
@@ -1531,7 +1531,7 @@
         <v>1150</v>
       </c>
       <c r="T16" s="25">
-        <v>45814</v>
+        <v>45846</v>
       </c>
       <c r="U16" s="26">
         <v>.2916666666666673352208</v>
@@ -1542,13 +1542,13 @@
         <v>63</v>
       </c>
       <c r="B17" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" s="8">
         <v>188</v>
       </c>
       <c r="D17" s="9">
-        <v>63</v>
+        <v>120</v>
       </c>
       <c r="E17" t="s" s="10">
         <v>56</v>
@@ -1578,7 +1578,7 @@
         <v>1500</v>
       </c>
       <c r="T17" s="25">
-        <v>45813</v>
+        <v>45846</v>
       </c>
       <c r="U17" s="26">
         <v>.2916666666666673352208</v>
@@ -1589,13 +1589,13 @@
         <v>65</v>
       </c>
       <c r="B18" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18" s="8">
         <v>146</v>
       </c>
       <c r="D18" s="9">
-        <v>63</v>
+        <v>120</v>
       </c>
       <c r="E18" t="s" s="10">
         <v>56</v>
@@ -1625,7 +1625,7 @@
         <v>1000</v>
       </c>
       <c r="T18" s="25">
-        <v>45817</v>
+        <v>45846</v>
       </c>
       <c r="U18" s="26">
         <v>.2916666666666673352208</v>

</xml_diff>

<commit_message>
Piccoli aggiustamenti pt. 4
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_input/Scheda_Macchine_Taglio.xlsx
+++ b/PS-VRP/Dati_input/Scheda_Macchine_Taglio.xlsx
@@ -9,7 +9,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t>Nome macchina</t>
   </si>
@@ -32,9 +32,6 @@
     <t>diam tubo ult lavoro</t>
   </si>
   <si>
-    <t>fascia ult lavoro</t>
-  </si>
-  <si>
     <t>Fascia min iniziale</t>
   </si>
   <si>
@@ -65,7 +62,7 @@
     <t>paranco</t>
   </si>
   <si>
-    <t>diametro finale max</t>
+    <t>diametro finale</t>
   </si>
   <si>
     <t>Fascia min finale</t>
@@ -219,16 +216,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="33">
+  <numFmts count="32">
     <numFmt formatCode="@" numFmtId="165"/>
     <numFmt formatCode="mm/dd/yyyy" numFmtId="166"/>
     <numFmt formatCode="[hh]:mm:ss" numFmtId="167"/>
     <numFmt formatCode="@" numFmtId="168"/>
     <numFmt formatCode="@" numFmtId="172"/>
-    <numFmt formatCode="@" numFmtId="179"/>
-    <numFmt formatCode="@" numFmtId="185"/>
-    <numFmt formatCode="dd/mm/yyyy" numFmtId="188"/>
-    <numFmt formatCode="[hh]:mm:ss" numFmtId="189"/>
+    <numFmt formatCode="@" numFmtId="178"/>
+    <numFmt formatCode="@" numFmtId="184"/>
+    <numFmt formatCode="dd/mm/yyyy" numFmtId="187"/>
+    <numFmt formatCode="[hh]:mm:ss" numFmtId="188"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -264,7 +261,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -309,40 +306,37 @@
     <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="top"/>
-    </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="179" xfId="0">
-      <alignment horizontal="general" vertical="top"/>
-    </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="top"/>
-    </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="top"/>
-    </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="top"/>
-    </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="top"/>
-    </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="top"/>
-    </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="185" xfId="0">
-      <alignment horizontal="general" vertical="top"/>
-    </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="top"/>
-    </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="178" xfId="0">
+      <alignment horizontal="general" vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="general" vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="general" vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="general" vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="general" vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="general" vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="184" xfId="0">
+      <alignment horizontal="general" vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="general" vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="general" vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="187" xfId="0">
       <alignment horizontal="general" vertical="top"/>
     </xf>
     <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="188" xfId="0">
-      <alignment horizontal="general" vertical="top"/>
-    </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="189" xfId="0">
       <alignment horizontal="general" vertical="top"/>
     </xf>
     <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
@@ -459,13 +453,10 @@
       <c r="AB1" t="s" s="1">
         <v>27</v>
       </c>
-      <c r="AC1" t="s" s="1">
-        <v>28</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="6">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="7">
         <v>0</v>
@@ -477,46 +468,55 @@
         <v>120</v>
       </c>
       <c r="E2" t="s" s="10">
+        <v>29</v>
+      </c>
+      <c r="F2" s="11">
+        <v>5</v>
+      </c>
+      <c r="G2" s="12">
+        <v>70</v>
+      </c>
+      <c r="H2" s="13">
+        <v>450</v>
+      </c>
+      <c r="I2" s="14">
+        <v>1</v>
+      </c>
+      <c r="J2" s="15">
+        <v>1200</v>
+      </c>
+      <c r="K2" t="s" s="16">
         <v>30</v>
       </c>
-      <c r="I2" s="14">
-        <v>450</v>
-      </c>
-      <c r="J2" s="15">
-        <v>1</v>
-      </c>
-      <c r="K2" s="16">
+      <c r="L2" s="17">
         <v>1200</v>
       </c>
-      <c r="L2" t="s" s="17">
+      <c r="O2" s="20">
+        <v>8</v>
+      </c>
+      <c r="P2" s="21">
+        <v>1200</v>
+      </c>
+      <c r="Q2" t="s" s="22">
         <v>31</v>
       </c>
-      <c r="M2" s="18">
-        <v>1200</v>
-      </c>
-      <c r="P2" s="21">
-        <v>8</v>
-      </c>
-      <c r="Q2" s="22">
-        <v>1200</v>
-      </c>
-      <c r="R2" t="s" s="23">
-        <v>32</v>
-      </c>
-      <c r="S2" s="24">
+      <c r="R2" s="23">
         <v>500</v>
       </c>
+      <c r="T2" s="25">
+        <v>45846</v>
+      </c>
       <c r="U2" s="26">
-        <v>45846</v>
+        <v>.2916666666666673352208</v>
       </c>
       <c r="V2" s="27">
-        <v>.5000000000000011460928</v>
+        <v>20</v>
       </c>
       <c r="W2" s="28">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="X2" s="29">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="Y2" s="30">
         <v>5</v>
@@ -525,18 +525,15 @@
         <v>5</v>
       </c>
       <c r="AA2" s="32">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AB2" s="33">
-        <v>0</v>
-      </c>
-      <c r="AC2" s="34">
         <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="6">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" s="7">
         <v>1</v>
@@ -548,7 +545,7 @@
         <v>120</v>
       </c>
       <c r="E3" t="s" s="10">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F3" s="11">
         <v>3</v>
@@ -557,69 +554,66 @@
         <v>76</v>
       </c>
       <c r="H3" s="13">
-        <v>285</v>
+        <v>400</v>
       </c>
       <c r="I3" s="14">
-        <v>400</v>
+        <v>2</v>
       </c>
       <c r="J3" s="15">
+        <v>1350</v>
+      </c>
+      <c r="K3" t="s" s="16">
+        <v>33</v>
+      </c>
+      <c r="L3" s="17">
+        <v>800</v>
+      </c>
+      <c r="O3" s="20">
+        <v>13</v>
+      </c>
+      <c r="P3" s="21">
+        <v>1000</v>
+      </c>
+      <c r="Q3" t="s" s="22">
+        <v>34</v>
+      </c>
+      <c r="R3" s="23">
+        <v>500</v>
+      </c>
+      <c r="S3" s="24">
+        <v>50</v>
+      </c>
+      <c r="T3" s="25">
+        <v>45846</v>
+      </c>
+      <c r="U3" s="26">
+        <v>.2916666666666673352208</v>
+      </c>
+      <c r="V3" s="27">
+        <v>15</v>
+      </c>
+      <c r="W3" s="28">
+        <v>5</v>
+      </c>
+      <c r="X3" s="29">
         <v>2</v>
       </c>
-      <c r="K3" s="16">
-        <v>1350</v>
-      </c>
-      <c r="L3" t="s" s="17">
-        <v>34</v>
-      </c>
-      <c r="M3" s="18">
-        <v>800</v>
-      </c>
-      <c r="P3" s="21">
-        <v>13</v>
-      </c>
-      <c r="Q3" s="22">
-        <v>1000</v>
-      </c>
-      <c r="R3" t="s" s="23">
-        <v>35</v>
-      </c>
-      <c r="S3" s="24">
-        <v>500</v>
-      </c>
-      <c r="T3" s="25">
-        <v>50</v>
-      </c>
-      <c r="U3" s="26">
-        <v>45846</v>
-      </c>
-      <c r="V3" s="27">
-        <v>.5000000000000011460928</v>
-      </c>
-      <c r="W3" s="28">
-        <v>15</v>
-      </c>
-      <c r="X3" s="29">
-        <v>5</v>
-      </c>
       <c r="Y3" s="30">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="Z3" s="31">
         <v>5</v>
       </c>
       <c r="AA3" s="32">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AB3" s="33">
-        <v>0</v>
-      </c>
-      <c r="AC3" s="34">
         <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="6">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" s="7">
         <v>0</v>
@@ -631,7 +625,7 @@
         <v>120</v>
       </c>
       <c r="E4" t="s" s="10">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F4" s="11">
         <v>5</v>
@@ -640,69 +634,66 @@
         <v>70</v>
       </c>
       <c r="H4" s="13">
-        <v>138</v>
+        <v>400</v>
       </c>
       <c r="I4" s="14">
-        <v>400</v>
+        <v>3</v>
       </c>
       <c r="J4" s="15">
-        <v>3</v>
-      </c>
-      <c r="K4" s="16">
         <v>1350</v>
       </c>
-      <c r="L4" t="s" s="17">
-        <v>37</v>
-      </c>
-      <c r="M4" s="18">
+      <c r="K4" t="s" s="16">
+        <v>36</v>
+      </c>
+      <c r="L4" s="17">
         <v>800</v>
       </c>
+      <c r="O4" s="20">
+        <v>13</v>
+      </c>
       <c r="P4" s="21">
-        <v>13</v>
-      </c>
-      <c r="Q4" s="22">
         <v>1000</v>
       </c>
-      <c r="R4" t="s" s="23">
-        <v>32</v>
+      <c r="Q4" t="s" s="22">
+        <v>31</v>
+      </c>
+      <c r="R4" s="23">
+        <v>500</v>
       </c>
       <c r="S4" s="24">
-        <v>500</v>
+        <v>50</v>
       </c>
       <c r="T4" s="25">
-        <v>50</v>
+        <v>45846</v>
       </c>
       <c r="U4" s="26">
-        <v>45846</v>
+        <v>.2916666666666673352208</v>
       </c>
       <c r="V4" s="27">
-        <v>.5000000000000011460928</v>
+        <v>15</v>
       </c>
       <c r="W4" s="28">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="X4" s="29">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="Y4" s="30">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="Z4" s="31">
         <v>5</v>
       </c>
       <c r="AA4" s="32">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AB4" s="33">
-        <v>0</v>
-      </c>
-      <c r="AC4" s="34">
         <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="6">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="7">
         <v>1</v>
@@ -714,78 +705,75 @@
         <v>120</v>
       </c>
       <c r="E5" t="s" s="10">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F5" s="11">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G5" s="12">
         <v>76</v>
       </c>
       <c r="H5" s="13">
-        <v>420</v>
+        <v>400</v>
       </c>
       <c r="I5" s="14">
-        <v>400</v>
+        <v>4</v>
       </c>
       <c r="J5" s="15">
-        <v>4</v>
-      </c>
-      <c r="K5" s="16">
         <v>1350</v>
       </c>
-      <c r="L5" t="s" s="17">
-        <v>39</v>
-      </c>
-      <c r="M5" s="18">
+      <c r="K5" t="s" s="16">
+        <v>38</v>
+      </c>
+      <c r="L5" s="17">
         <v>800</v>
       </c>
+      <c r="O5" s="20">
+        <v>10</v>
+      </c>
       <c r="P5" s="21">
-        <v>10</v>
-      </c>
-      <c r="Q5" s="22">
         <v>1200</v>
       </c>
-      <c r="R5" t="s" s="23">
-        <v>32</v>
+      <c r="Q5" t="s" s="22">
+        <v>31</v>
+      </c>
+      <c r="R5" s="23">
+        <v>500</v>
       </c>
       <c r="S5" s="24">
-        <v>500</v>
+        <v>50</v>
       </c>
       <c r="T5" s="25">
-        <v>50</v>
+        <v>45846</v>
       </c>
       <c r="U5" s="26">
-        <v>45846</v>
+        <v>.2916666666666673352208</v>
       </c>
       <c r="V5" s="27">
-        <v>.5000000000000011460928</v>
+        <v>15</v>
       </c>
       <c r="W5" s="28">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="X5" s="29">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="Y5" s="30">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="Z5" s="31">
         <v>5</v>
       </c>
       <c r="AA5" s="32">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AB5" s="33">
-        <v>0</v>
-      </c>
-      <c r="AC5" s="34">
         <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="6">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6" s="7">
         <v>1</v>
@@ -797,75 +785,72 @@
         <v>120</v>
       </c>
       <c r="E6" t="s" s="10">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F6" s="11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G6" s="12">
         <v>70</v>
       </c>
       <c r="H6" s="13">
-        <v>225</v>
+        <v>400</v>
       </c>
       <c r="I6" s="14">
-        <v>400</v>
+        <v>5</v>
       </c>
       <c r="J6" s="15">
-        <v>5</v>
-      </c>
-      <c r="K6" s="16">
         <v>1100</v>
       </c>
-      <c r="L6" t="s" s="17">
-        <v>41</v>
-      </c>
-      <c r="M6" s="18">
+      <c r="K6" t="s" s="16">
+        <v>40</v>
+      </c>
+      <c r="L6" s="17">
         <v>800</v>
       </c>
+      <c r="O6" s="20">
+        <v>14</v>
+      </c>
       <c r="P6" s="21">
-        <v>14</v>
-      </c>
-      <c r="Q6" s="22">
         <v>1000</v>
       </c>
-      <c r="R6" t="s" s="23">
-        <v>32</v>
-      </c>
-      <c r="S6" s="24">
+      <c r="Q6" t="s" s="22">
+        <v>31</v>
+      </c>
+      <c r="R6" s="23">
         <v>500</v>
       </c>
+      <c r="T6" s="25">
+        <v>45846</v>
+      </c>
       <c r="U6" s="26">
-        <v>45846</v>
+        <v>.2916666666666673352208</v>
       </c>
       <c r="V6" s="27">
-        <v>.5000000000000011460928</v>
+        <v>0</v>
       </c>
       <c r="W6" s="28">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="X6" s="29">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="Y6" s="30">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="Z6" s="31">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="AA6" s="32">
-        <v>10</v>
+        <v>.5</v>
       </c>
       <c r="AB6" s="33">
-        <v>.5</v>
-      </c>
-      <c r="AC6" s="34">
         <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="6">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" s="7">
         <v>0</v>
@@ -877,55 +862,55 @@
         <v>120</v>
       </c>
       <c r="E7" t="s" s="10">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F7" s="11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G7" s="12">
         <v>70</v>
       </c>
       <c r="H7" s="13">
-        <v>280</v>
+        <v>20</v>
       </c>
       <c r="I7" s="14">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="J7" s="15">
-        <v>6</v>
-      </c>
-      <c r="K7" s="16">
         <v>1050</v>
       </c>
-      <c r="L7" t="s" s="17">
-        <v>43</v>
-      </c>
-      <c r="M7" s="18">
+      <c r="K7" t="s" s="16">
+        <v>42</v>
+      </c>
+      <c r="L7" s="17">
         <v>750</v>
       </c>
+      <c r="O7" s="20">
+        <v>8</v>
+      </c>
       <c r="P7" s="21">
-        <v>8</v>
-      </c>
-      <c r="Q7" s="22">
         <v>1050</v>
       </c>
-      <c r="R7" t="s" s="23">
-        <v>32</v>
-      </c>
-      <c r="S7" s="24">
+      <c r="Q7" t="s" s="22">
+        <v>31</v>
+      </c>
+      <c r="R7" s="23">
         <v>420</v>
       </c>
+      <c r="T7" s="25">
+        <v>45846</v>
+      </c>
       <c r="U7" s="26">
-        <v>45846</v>
+        <v>.2916666666666673352208</v>
       </c>
       <c r="V7" s="27">
-        <v>.5000000000000011460928</v>
+        <v>2</v>
       </c>
       <c r="W7" s="28">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="X7" s="29">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="Y7" s="30">
         <v>5</v>
@@ -937,15 +922,12 @@
         <v>5</v>
       </c>
       <c r="AB7" s="33">
-        <v>5</v>
-      </c>
-      <c r="AC7" s="34">
         <v>5</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="6">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="7">
         <v>1</v>
@@ -957,78 +939,72 @@
         <v>120</v>
       </c>
       <c r="E8" t="s" s="10">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F8" s="11">
-        <v>2</v>
-      </c>
-      <c r="G8" s="12">
-        <v>76</v>
+        <v>1</v>
       </c>
       <c r="H8" s="13">
         <v>400</v>
       </c>
       <c r="I8" s="14">
-        <v>400</v>
+        <v>7</v>
       </c>
       <c r="J8" s="15">
-        <v>7</v>
-      </c>
-      <c r="K8" s="16">
         <v>1350</v>
       </c>
-      <c r="L8" t="s" s="17">
-        <v>45</v>
-      </c>
-      <c r="M8" s="18">
+      <c r="K8" t="s" s="16">
+        <v>44</v>
+      </c>
+      <c r="L8" s="17">
         <v>800</v>
       </c>
+      <c r="O8" s="20">
+        <v>10</v>
+      </c>
       <c r="P8" s="21">
-        <v>10</v>
-      </c>
-      <c r="Q8" s="22">
         <v>1000</v>
       </c>
-      <c r="R8" t="s" s="23">
-        <v>32</v>
+      <c r="Q8" t="s" s="22">
+        <v>31</v>
+      </c>
+      <c r="R8" s="23">
+        <v>500</v>
       </c>
       <c r="S8" s="24">
-        <v>500</v>
+        <v>50</v>
       </c>
       <c r="T8" s="25">
-        <v>50</v>
+        <v>45846</v>
       </c>
       <c r="U8" s="26">
-        <v>45846</v>
+        <v>.2916666666666673352208</v>
       </c>
       <c r="V8" s="27">
-        <v>.5000000000000011460928</v>
+        <v>15</v>
       </c>
       <c r="W8" s="28">
         <v>15</v>
       </c>
       <c r="X8" s="29">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="Y8" s="30">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="Z8" s="31">
         <v>5</v>
       </c>
       <c r="AA8" s="32">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AB8" s="33">
-        <v>0</v>
-      </c>
-      <c r="AC8" s="34">
         <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="6">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" s="7">
         <v>1</v>
@@ -1040,52 +1016,55 @@
         <v>120</v>
       </c>
       <c r="E9" t="s" s="10">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F9" s="11">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="G9" s="12">
+        <v>70</v>
       </c>
       <c r="H9" s="13">
-        <v>286</v>
+        <v>0</v>
       </c>
       <c r="I9" s="14">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J9" s="15">
-        <v>8</v>
-      </c>
-      <c r="K9" s="16">
         <v>1300</v>
       </c>
-      <c r="L9" t="s" s="17">
-        <v>47</v>
-      </c>
-      <c r="M9" s="18">
+      <c r="K9" t="s" s="16">
+        <v>46</v>
+      </c>
+      <c r="L9" s="17">
         <v>1000</v>
       </c>
+      <c r="O9" s="20">
+        <v>10</v>
+      </c>
       <c r="P9" s="21">
+        <v>1260</v>
+      </c>
+      <c r="Q9" t="s" s="22">
+        <v>34</v>
+      </c>
+      <c r="R9" s="23">
+        <v>600</v>
+      </c>
+      <c r="T9" s="25">
+        <v>45846</v>
+      </c>
+      <c r="U9" s="26">
+        <v>.2916666666666673352208</v>
+      </c>
+      <c r="V9" s="27">
+        <v>5</v>
+      </c>
+      <c r="W9" s="28">
         <v>10</v>
       </c>
-      <c r="Q9" s="22">
-        <v>1260</v>
-      </c>
-      <c r="R9" t="s" s="23">
-        <v>35</v>
-      </c>
-      <c r="S9" s="24">
-        <v>600</v>
-      </c>
-      <c r="U9" s="26">
-        <v>45846</v>
-      </c>
-      <c r="V9" s="27">
-        <v>.5000000000000011460928</v>
-      </c>
-      <c r="W9" s="28">
-        <v>5</v>
-      </c>
       <c r="X9" s="29">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="Y9" s="30">
         <v>5</v>
@@ -1097,15 +1076,12 @@
         <v>5</v>
       </c>
       <c r="AB9" s="33">
-        <v>5</v>
-      </c>
-      <c r="AC9" s="34">
         <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="6">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B10" s="7">
         <v>0</v>
@@ -1117,49 +1093,58 @@
         <v>120</v>
       </c>
       <c r="E10" t="s" s="10">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="F10" s="11">
+        <v>4</v>
+      </c>
+      <c r="G10" s="12">
+        <v>70</v>
+      </c>
+      <c r="H10" s="13">
+        <v>0</v>
       </c>
       <c r="I10" s="14">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J10" s="15">
-        <v>9</v>
-      </c>
-      <c r="K10" s="16">
         <v>910</v>
       </c>
-      <c r="L10" t="s" s="17">
-        <v>49</v>
-      </c>
-      <c r="M10" s="18">
+      <c r="K10" t="s" s="16">
+        <v>48</v>
+      </c>
+      <c r="L10" s="17">
         <v>620</v>
       </c>
+      <c r="O10" s="20">
+        <v>37</v>
+      </c>
       <c r="P10" s="21">
-        <v>37</v>
-      </c>
-      <c r="Q10" s="22">
         <v>900</v>
       </c>
-      <c r="R10" t="s" s="23">
-        <v>35</v>
+      <c r="Q10" t="s" s="22">
+        <v>34</v>
+      </c>
+      <c r="R10" s="23">
+        <v>450</v>
       </c>
       <c r="S10" s="24">
-        <v>450</v>
+        <v>18</v>
       </c>
       <c r="T10" s="25">
-        <v>18</v>
+        <v>45846</v>
       </c>
       <c r="U10" s="26">
-        <v>45846</v>
+        <v>.2916666666666673352208</v>
       </c>
       <c r="V10" s="27">
-        <v>.5000000000000011460928</v>
+        <v>2</v>
       </c>
       <c r="W10" s="28">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="X10" s="29">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="Y10" s="30">
         <v>5</v>
@@ -1171,15 +1156,12 @@
         <v>5</v>
       </c>
       <c r="AB10" s="33">
-        <v>5</v>
-      </c>
-      <c r="AC10" s="34">
         <v>5</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="6">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B11" s="7">
         <v>1</v>
@@ -1191,58 +1173,58 @@
         <v>120</v>
       </c>
       <c r="E11" t="s" s="10">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F11" s="11">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="G11" s="12">
         <v>70</v>
       </c>
       <c r="H11" s="13">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I11" s="14">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J11" s="15">
+        <v>1080</v>
+      </c>
+      <c r="K11" t="s" s="16">
+        <v>50</v>
+      </c>
+      <c r="L11" s="17">
+        <v>800</v>
+      </c>
+      <c r="O11" s="20">
+        <v>24</v>
+      </c>
+      <c r="P11" s="21">
+        <v>530</v>
+      </c>
+      <c r="Q11" t="s" s="22">
+        <v>31</v>
+      </c>
+      <c r="R11" s="23">
+        <v>600</v>
+      </c>
+      <c r="S11" s="24">
+        <v>40</v>
+      </c>
+      <c r="T11" s="25">
+        <v>45846</v>
+      </c>
+      <c r="U11" s="26">
+        <v>.2916666666666673352208</v>
+      </c>
+      <c r="V11" s="27">
         <v>10</v>
-      </c>
-      <c r="K11" s="16">
-        <v>1080</v>
-      </c>
-      <c r="L11" t="s" s="17">
-        <v>51</v>
-      </c>
-      <c r="M11" s="18">
-        <v>800</v>
-      </c>
-      <c r="P11" s="21">
-        <v>24</v>
-      </c>
-      <c r="Q11" s="22">
-        <v>530</v>
-      </c>
-      <c r="R11" t="s" s="23">
-        <v>32</v>
-      </c>
-      <c r="S11" s="24">
-        <v>600</v>
-      </c>
-      <c r="T11" s="25">
-        <v>40</v>
-      </c>
-      <c r="U11" s="26">
-        <v>45846</v>
-      </c>
-      <c r="V11" s="27">
-        <v>.5000000000000011460928</v>
       </c>
       <c r="W11" s="28">
         <v>10</v>
       </c>
       <c r="X11" s="29">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="Y11" s="30">
         <v>5</v>
@@ -1254,15 +1236,12 @@
         <v>5</v>
       </c>
       <c r="AB11" s="33">
-        <v>5</v>
-      </c>
-      <c r="AC11" s="34">
         <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="6">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B12" s="7">
         <v>1</v>
@@ -1274,7 +1253,7 @@
         <v>120</v>
       </c>
       <c r="E12" t="s" s="10">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F12" s="11">
         <v>3</v>
@@ -1283,46 +1262,46 @@
         <v>152</v>
       </c>
       <c r="H12" s="13">
-        <v>408</v>
+        <v>0</v>
       </c>
       <c r="I12" s="14">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="J12" s="15">
-        <v>11</v>
-      </c>
-      <c r="K12" s="16">
         <v>1300</v>
       </c>
-      <c r="L12" t="s" s="17">
-        <v>53</v>
-      </c>
-      <c r="M12" s="18">
+      <c r="K12" t="s" s="16">
+        <v>52</v>
+      </c>
+      <c r="L12" s="17">
         <v>1000</v>
       </c>
+      <c r="O12" s="20">
+        <v>10</v>
+      </c>
       <c r="P12" s="21">
+        <v>1260</v>
+      </c>
+      <c r="Q12" t="s" s="22">
+        <v>34</v>
+      </c>
+      <c r="R12" s="23">
+        <v>600</v>
+      </c>
+      <c r="T12" s="25">
+        <v>45846</v>
+      </c>
+      <c r="U12" s="26">
+        <v>.2916666666666673352208</v>
+      </c>
+      <c r="V12" s="27">
+        <v>5</v>
+      </c>
+      <c r="W12" s="28">
         <v>10</v>
       </c>
-      <c r="Q12" s="22">
-        <v>1260</v>
-      </c>
-      <c r="R12" t="s" s="23">
-        <v>35</v>
-      </c>
-      <c r="S12" s="24">
-        <v>600</v>
-      </c>
-      <c r="U12" s="26">
-        <v>45846</v>
-      </c>
-      <c r="V12" s="27">
-        <v>.5000000000000011460928</v>
-      </c>
-      <c r="W12" s="28">
-        <v>5</v>
-      </c>
       <c r="X12" s="29">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="Y12" s="30">
         <v>5</v>
@@ -1334,15 +1313,12 @@
         <v>5</v>
       </c>
       <c r="AB12" s="33">
-        <v>5</v>
-      </c>
-      <c r="AC12" s="34">
         <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="6">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B13" s="7">
         <v>1</v>
@@ -1354,7 +1330,7 @@
         <v>120</v>
       </c>
       <c r="E13" t="s" s="10">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F13" s="11">
         <v>2</v>
@@ -1363,69 +1339,66 @@
         <v>76</v>
       </c>
       <c r="H13" s="13">
-        <v>480</v>
+        <v>400</v>
       </c>
       <c r="I13" s="14">
-        <v>400</v>
+        <v>12</v>
       </c>
       <c r="J13" s="15">
-        <v>12</v>
-      </c>
-      <c r="K13" s="16">
         <v>1350</v>
       </c>
-      <c r="L13" t="s" s="17">
-        <v>55</v>
-      </c>
-      <c r="M13" s="18">
+      <c r="K13" t="s" s="16">
+        <v>54</v>
+      </c>
+      <c r="L13" s="17">
         <v>800</v>
       </c>
+      <c r="O13" s="20">
+        <v>10</v>
+      </c>
       <c r="P13" s="21">
-        <v>10</v>
-      </c>
-      <c r="Q13" s="22">
         <v>1000</v>
       </c>
-      <c r="R13" t="s" s="23">
-        <v>35</v>
+      <c r="Q13" t="s" s="22">
+        <v>34</v>
+      </c>
+      <c r="R13" s="23">
+        <v>500</v>
       </c>
       <c r="S13" s="24">
-        <v>500</v>
+        <v>50</v>
       </c>
       <c r="T13" s="25">
-        <v>50</v>
+        <v>45846</v>
       </c>
       <c r="U13" s="26">
-        <v>45846</v>
+        <v>.2916666666666673352208</v>
       </c>
       <c r="V13" s="27">
-        <v>.5000000000000011460928</v>
+        <v>15</v>
       </c>
       <c r="W13" s="28">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="X13" s="29">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="Y13" s="30">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="Z13" s="31">
         <v>5</v>
       </c>
       <c r="AA13" s="32">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AB13" s="33">
-        <v>0</v>
-      </c>
-      <c r="AC13" s="34">
         <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="6">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B14" s="7">
         <v>0</v>
@@ -1437,42 +1410,42 @@
         <v>120</v>
       </c>
       <c r="E14" t="s" s="10">
+        <v>56</v>
+      </c>
+      <c r="F14" t="s" s="11">
         <v>57</v>
       </c>
-      <c r="F14" t="s" s="11">
+      <c r="H14" s="13">
+        <v>0</v>
+      </c>
+      <c r="I14" s="14">
+        <v>13</v>
+      </c>
+      <c r="J14" s="15">
+        <v>810</v>
+      </c>
+      <c r="K14" t="s" s="16">
         <v>58</v>
       </c>
-      <c r="I14" s="14">
-        <v>0</v>
-      </c>
-      <c r="J14" s="15">
-        <v>13</v>
-      </c>
-      <c r="K14" s="16">
-        <v>810</v>
-      </c>
-      <c r="L14" t="s" s="17">
-        <v>59</v>
+      <c r="L14" s="17">
+        <v>800</v>
       </c>
       <c r="M14" s="18">
-        <v>800</v>
+        <v>330</v>
       </c>
       <c r="N14" s="19">
-        <v>330</v>
-      </c>
-      <c r="O14" s="20">
         <v>640</v>
       </c>
+      <c r="T14" s="25">
+        <v>45846</v>
+      </c>
       <c r="U14" s="26">
-        <v>45846</v>
-      </c>
-      <c r="V14" s="27">
-        <v>.5000000000000011460928</v>
+        <v>.2916666666666673352208</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="6">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B15" s="7">
         <v>0</v>
@@ -1484,39 +1457,42 @@
         <v>120</v>
       </c>
       <c r="E15" t="s" s="10">
+        <v>56</v>
+      </c>
+      <c r="F15" t="s" s="11">
         <v>57</v>
       </c>
+      <c r="H15" s="13">
+        <v>0</v>
+      </c>
       <c r="I15" s="14">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="J15" s="15">
-        <v>14</v>
-      </c>
-      <c r="K15" s="16">
         <v>1050</v>
       </c>
-      <c r="L15" t="s" s="17">
-        <v>61</v>
+      <c r="K15" t="s" s="16">
+        <v>60</v>
+      </c>
+      <c r="L15" s="17">
+        <v>800</v>
       </c>
       <c r="M15" s="18">
-        <v>800</v>
+        <v>400</v>
       </c>
       <c r="N15" s="19">
-        <v>400</v>
-      </c>
-      <c r="O15" s="20">
         <v>1000</v>
       </c>
+      <c r="T15" s="25">
+        <v>45846</v>
+      </c>
       <c r="U15" s="26">
-        <v>45846</v>
-      </c>
-      <c r="V15" s="27">
-        <v>.5000000000000011460928</v>
+        <v>.2916666666666673352208</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="6">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B16" s="7">
         <v>0</v>
@@ -1528,42 +1504,42 @@
         <v>120</v>
       </c>
       <c r="E16" t="s" s="10">
+        <v>56</v>
+      </c>
+      <c r="F16" t="s" s="11">
         <v>57</v>
       </c>
-      <c r="F16" t="s" s="11">
-        <v>58</v>
+      <c r="H16" s="13">
+        <v>0</v>
       </c>
       <c r="I16" s="14">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="J16" s="15">
-        <v>15</v>
-      </c>
-      <c r="K16" s="16">
         <v>910</v>
       </c>
-      <c r="L16" t="s" s="17">
-        <v>63</v>
+      <c r="K16" t="s" s="16">
+        <v>62</v>
+      </c>
+      <c r="L16" s="17">
+        <v>800</v>
       </c>
       <c r="M16" s="18">
-        <v>800</v>
+        <v>300</v>
       </c>
       <c r="N16" s="19">
-        <v>300</v>
-      </c>
-      <c r="O16" s="20">
         <v>1150</v>
       </c>
+      <c r="T16" s="25">
+        <v>45846</v>
+      </c>
       <c r="U16" s="26">
-        <v>45846</v>
-      </c>
-      <c r="V16" s="27">
-        <v>.5000000000000011460928</v>
+        <v>.2916666666666673352208</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="6">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B17" s="7">
         <v>0</v>
@@ -1575,39 +1551,42 @@
         <v>120</v>
       </c>
       <c r="E17" t="s" s="10">
+        <v>56</v>
+      </c>
+      <c r="F17" t="s" s="11">
         <v>57</v>
       </c>
+      <c r="H17" s="13">
+        <v>0</v>
+      </c>
       <c r="I17" s="14">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J17" s="15">
-        <v>16</v>
-      </c>
-      <c r="K17" s="16">
         <v>1220</v>
       </c>
-      <c r="L17" t="s" s="17">
-        <v>65</v>
+      <c r="K17" t="s" s="16">
+        <v>64</v>
+      </c>
+      <c r="L17" s="17">
+        <v>800</v>
       </c>
       <c r="M17" s="18">
-        <v>800</v>
+        <v>400</v>
       </c>
       <c r="N17" s="19">
-        <v>400</v>
-      </c>
-      <c r="O17" s="20">
         <v>1500</v>
       </c>
+      <c r="T17" s="25">
+        <v>45846</v>
+      </c>
       <c r="U17" s="26">
-        <v>45846</v>
-      </c>
-      <c r="V17" s="27">
-        <v>.5000000000000011460928</v>
+        <v>.2916666666666673352208</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="6">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B18" s="7">
         <v>0</v>
@@ -1619,37 +1598,37 @@
         <v>120</v>
       </c>
       <c r="E18" t="s" s="10">
+        <v>56</v>
+      </c>
+      <c r="F18" t="s" s="11">
         <v>57</v>
       </c>
-      <c r="F18" t="s" s="11">
-        <v>58</v>
+      <c r="H18" s="13">
+        <v>0</v>
       </c>
       <c r="I18" s="14">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="J18" s="15">
-        <v>17</v>
-      </c>
-      <c r="K18" s="16">
         <v>1050</v>
       </c>
-      <c r="L18" t="s" s="17">
-        <v>67</v>
+      <c r="K18" t="s" s="16">
+        <v>66</v>
+      </c>
+      <c r="L18" s="17">
+        <v>800</v>
       </c>
       <c r="M18" s="18">
-        <v>800</v>
+        <v>400</v>
       </c>
       <c r="N18" s="19">
-        <v>400</v>
-      </c>
-      <c r="O18" s="20">
         <v>1000</v>
       </c>
+      <c r="T18" s="25">
+        <v>45846</v>
+      </c>
       <c r="U18" s="26">
-        <v>45846</v>
-      </c>
-      <c r="V18" s="27">
-        <v>.5000000000000011460928</v>
+        <v>.2916666666666673352208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambiata folder structure file input
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_input/Scheda_Macchine_Taglio.xlsx
+++ b/PS-VRP/Dati_input/Scheda_Macchine_Taglio.xlsx
@@ -9,7 +9,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t>Nome macchina</t>
   </si>
@@ -32,6 +32,9 @@
     <t>diam tubo ult lavoro</t>
   </si>
   <si>
+    <t>fascia ult lavoro</t>
+  </si>
+  <si>
     <t>Fascia min iniziale</t>
   </si>
   <si>
@@ -62,7 +65,7 @@
     <t>paranco</t>
   </si>
   <si>
-    <t>diametro finale</t>
+    <t>diametro finale max</t>
   </si>
   <si>
     <t>Fascia min finale</t>
@@ -216,16 +219,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="32">
+  <numFmts count="33">
     <numFmt formatCode="@" numFmtId="165"/>
     <numFmt formatCode="mm/dd/yyyy" numFmtId="166"/>
     <numFmt formatCode="[hh]:mm:ss" numFmtId="167"/>
     <numFmt formatCode="@" numFmtId="168"/>
     <numFmt formatCode="@" numFmtId="172"/>
-    <numFmt formatCode="@" numFmtId="178"/>
-    <numFmt formatCode="@" numFmtId="184"/>
-    <numFmt formatCode="dd/mm/yyyy" numFmtId="187"/>
-    <numFmt formatCode="[hh]:mm:ss" numFmtId="188"/>
+    <numFmt formatCode="@" numFmtId="179"/>
+    <numFmt formatCode="@" numFmtId="185"/>
+    <numFmt formatCode="dd/mm/yyyy" numFmtId="188"/>
+    <numFmt formatCode="[hh]:mm:ss" numFmtId="189"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -261,7 +264,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -306,37 +309,40 @@
     <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="178" xfId="0">
-      <alignment horizontal="general" vertical="top"/>
-    </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="top"/>
-    </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="top"/>
-    </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="top"/>
-    </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="top"/>
-    </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="top"/>
-    </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="184" xfId="0">
-      <alignment horizontal="general" vertical="top"/>
-    </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="top"/>
-    </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="top"/>
-    </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="187" xfId="0">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="general" vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="179" xfId="0">
+      <alignment horizontal="general" vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="general" vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="general" vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="general" vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="general" vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="general" vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="185" xfId="0">
+      <alignment horizontal="general" vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="general" vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="top"/>
     </xf>
     <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="188" xfId="0">
+      <alignment horizontal="general" vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="189" xfId="0">
       <alignment horizontal="general" vertical="top"/>
     </xf>
     <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
@@ -453,10 +459,13 @@
       <c r="AB1" t="s" s="1">
         <v>27</v>
       </c>
+      <c r="AC1" t="s" s="1">
+        <v>28</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="6">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B2" s="7">
         <v>0</v>
@@ -468,56 +477,47 @@
         <v>120</v>
       </c>
       <c r="E2" t="s" s="10">
-        <v>29</v>
-      </c>
-      <c r="F2" s="11">
-        <v>5</v>
-      </c>
-      <c r="G2" s="12">
-        <v>70</v>
-      </c>
-      <c r="H2" s="13">
+        <v>30</v>
+      </c>
+      <c r="I2" s="14">
         <v>450</v>
       </c>
-      <c r="I2" s="14">
+      <c r="J2" s="15">
         <v>1</v>
       </c>
-      <c r="J2" s="15">
+      <c r="K2" s="16">
         <v>1200</v>
       </c>
-      <c r="K2" t="s" s="16">
-        <v>30</v>
-      </c>
-      <c r="L2" s="17">
+      <c r="L2" t="s" s="17">
+        <v>31</v>
+      </c>
+      <c r="M2" s="18">
         <v>1200</v>
       </c>
-      <c r="O2" s="20">
+      <c r="P2" s="21">
         <v>8</v>
       </c>
-      <c r="P2" s="21">
+      <c r="Q2" s="22">
         <v>1200</v>
       </c>
-      <c r="Q2" t="s" s="22">
-        <v>31</v>
-      </c>
-      <c r="R2" s="23">
+      <c r="R2" t="s" s="23">
+        <v>32</v>
+      </c>
+      <c r="S2" s="24">
         <v>500</v>
       </c>
-      <c r="T2" s="25">
+      <c r="U2" s="26">
         <v>45846</v>
       </c>
-      <c r="U2" s="26">
-        <v>.2916666666666673352208</v>
-      </c>
       <c r="V2" s="27">
+        <v>.5000000000000011460928</v>
+      </c>
+      <c r="W2" s="28">
         <v>20</v>
       </c>
-      <c r="W2" s="28">
+      <c r="X2" s="29">
         <v>10</v>
       </c>
-      <c r="X2" s="29">
-        <v>5</v>
-      </c>
       <c r="Y2" s="30">
         <v>5</v>
       </c>
@@ -525,15 +525,18 @@
         <v>5</v>
       </c>
       <c r="AA2" s="32">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AB2" s="33">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="34">
         <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="6">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B3" s="7">
         <v>1</v>
@@ -545,7 +548,7 @@
         <v>120</v>
       </c>
       <c r="E3" t="s" s="10">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F3" s="11">
         <v>3</v>
@@ -554,66 +557,69 @@
         <v>76</v>
       </c>
       <c r="H3" s="13">
+        <v>285</v>
+      </c>
+      <c r="I3" s="14">
         <v>400</v>
       </c>
-      <c r="I3" s="14">
+      <c r="J3" s="15">
         <v>2</v>
       </c>
-      <c r="J3" s="15">
+      <c r="K3" s="16">
         <v>1350</v>
       </c>
-      <c r="K3" t="s" s="16">
-        <v>33</v>
-      </c>
-      <c r="L3" s="17">
+      <c r="L3" t="s" s="17">
+        <v>34</v>
+      </c>
+      <c r="M3" s="18">
         <v>800</v>
       </c>
-      <c r="O3" s="20">
+      <c r="P3" s="21">
         <v>13</v>
       </c>
-      <c r="P3" s="21">
+      <c r="Q3" s="22">
         <v>1000</v>
       </c>
-      <c r="Q3" t="s" s="22">
-        <v>34</v>
-      </c>
-      <c r="R3" s="23">
+      <c r="R3" t="s" s="23">
+        <v>35</v>
+      </c>
+      <c r="S3" s="24">
         <v>500</v>
       </c>
-      <c r="S3" s="24">
+      <c r="T3" s="25">
         <v>50</v>
       </c>
-      <c r="T3" s="25">
+      <c r="U3" s="26">
         <v>45846</v>
       </c>
-      <c r="U3" s="26">
-        <v>.2916666666666673352208</v>
-      </c>
       <c r="V3" s="27">
+        <v>.5000000000000011460928</v>
+      </c>
+      <c r="W3" s="28">
         <v>15</v>
       </c>
-      <c r="W3" s="28">
-        <v>5</v>
-      </c>
       <c r="X3" s="29">
+        <v>5</v>
+      </c>
+      <c r="Y3" s="30">
         <v>2</v>
       </c>
-      <c r="Y3" s="30">
-        <v>5</v>
-      </c>
       <c r="Z3" s="31">
         <v>5</v>
       </c>
       <c r="AA3" s="32">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AB3" s="33">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="34">
         <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="6">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B4" s="7">
         <v>0</v>
@@ -625,7 +631,7 @@
         <v>120</v>
       </c>
       <c r="E4" t="s" s="10">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F4" s="11">
         <v>5</v>
@@ -634,66 +640,69 @@
         <v>70</v>
       </c>
       <c r="H4" s="13">
+        <v>138</v>
+      </c>
+      <c r="I4" s="14">
         <v>400</v>
       </c>
-      <c r="I4" s="14">
+      <c r="J4" s="15">
         <v>3</v>
       </c>
-      <c r="J4" s="15">
+      <c r="K4" s="16">
         <v>1350</v>
       </c>
-      <c r="K4" t="s" s="16">
-        <v>36</v>
-      </c>
-      <c r="L4" s="17">
+      <c r="L4" t="s" s="17">
+        <v>37</v>
+      </c>
+      <c r="M4" s="18">
         <v>800</v>
       </c>
-      <c r="O4" s="20">
+      <c r="P4" s="21">
         <v>13</v>
       </c>
-      <c r="P4" s="21">
+      <c r="Q4" s="22">
         <v>1000</v>
       </c>
-      <c r="Q4" t="s" s="22">
-        <v>31</v>
-      </c>
-      <c r="R4" s="23">
+      <c r="R4" t="s" s="23">
+        <v>32</v>
+      </c>
+      <c r="S4" s="24">
         <v>500</v>
       </c>
-      <c r="S4" s="24">
+      <c r="T4" s="25">
         <v>50</v>
       </c>
-      <c r="T4" s="25">
+      <c r="U4" s="26">
         <v>45846</v>
       </c>
-      <c r="U4" s="26">
-        <v>.2916666666666673352208</v>
-      </c>
       <c r="V4" s="27">
+        <v>.5000000000000011460928</v>
+      </c>
+      <c r="W4" s="28">
         <v>15</v>
       </c>
-      <c r="W4" s="28">
-        <v>5</v>
-      </c>
       <c r="X4" s="29">
+        <v>5</v>
+      </c>
+      <c r="Y4" s="30">
         <v>2</v>
       </c>
-      <c r="Y4" s="30">
-        <v>5</v>
-      </c>
       <c r="Z4" s="31">
         <v>5</v>
       </c>
       <c r="AA4" s="32">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AB4" s="33">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="34">
         <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="6">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B5" s="7">
         <v>1</v>
@@ -705,75 +714,78 @@
         <v>120</v>
       </c>
       <c r="E5" t="s" s="10">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F5" s="11">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G5" s="12">
         <v>76</v>
       </c>
       <c r="H5" s="13">
+        <v>420</v>
+      </c>
+      <c r="I5" s="14">
         <v>400</v>
       </c>
-      <c r="I5" s="14">
+      <c r="J5" s="15">
         <v>4</v>
       </c>
-      <c r="J5" s="15">
+      <c r="K5" s="16">
         <v>1350</v>
       </c>
-      <c r="K5" t="s" s="16">
-        <v>38</v>
-      </c>
-      <c r="L5" s="17">
+      <c r="L5" t="s" s="17">
+        <v>39</v>
+      </c>
+      <c r="M5" s="18">
         <v>800</v>
       </c>
-      <c r="O5" s="20">
+      <c r="P5" s="21">
         <v>10</v>
       </c>
-      <c r="P5" s="21">
+      <c r="Q5" s="22">
         <v>1200</v>
       </c>
-      <c r="Q5" t="s" s="22">
-        <v>31</v>
-      </c>
-      <c r="R5" s="23">
+      <c r="R5" t="s" s="23">
+        <v>32</v>
+      </c>
+      <c r="S5" s="24">
         <v>500</v>
       </c>
-      <c r="S5" s="24">
+      <c r="T5" s="25">
         <v>50</v>
       </c>
-      <c r="T5" s="25">
+      <c r="U5" s="26">
         <v>45846</v>
       </c>
-      <c r="U5" s="26">
-        <v>.2916666666666673352208</v>
-      </c>
       <c r="V5" s="27">
+        <v>.5000000000000011460928</v>
+      </c>
+      <c r="W5" s="28">
         <v>15</v>
       </c>
-      <c r="W5" s="28">
-        <v>5</v>
-      </c>
       <c r="X5" s="29">
+        <v>5</v>
+      </c>
+      <c r="Y5" s="30">
         <v>2</v>
       </c>
-      <c r="Y5" s="30">
-        <v>5</v>
-      </c>
       <c r="Z5" s="31">
         <v>5</v>
       </c>
       <c r="AA5" s="32">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AB5" s="33">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="34">
         <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="6">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B6" s="7">
         <v>1</v>
@@ -785,72 +797,75 @@
         <v>120</v>
       </c>
       <c r="E6" t="s" s="10">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F6" s="11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G6" s="12">
         <v>70</v>
       </c>
       <c r="H6" s="13">
+        <v>225</v>
+      </c>
+      <c r="I6" s="14">
         <v>400</v>
       </c>
-      <c r="I6" s="14">
-        <v>5</v>
-      </c>
       <c r="J6" s="15">
+        <v>5</v>
+      </c>
+      <c r="K6" s="16">
         <v>1100</v>
       </c>
-      <c r="K6" t="s" s="16">
-        <v>40</v>
-      </c>
-      <c r="L6" s="17">
+      <c r="L6" t="s" s="17">
+        <v>41</v>
+      </c>
+      <c r="M6" s="18">
         <v>800</v>
       </c>
-      <c r="O6" s="20">
+      <c r="P6" s="21">
         <v>14</v>
       </c>
-      <c r="P6" s="21">
+      <c r="Q6" s="22">
         <v>1000</v>
       </c>
-      <c r="Q6" t="s" s="22">
-        <v>31</v>
-      </c>
-      <c r="R6" s="23">
+      <c r="R6" t="s" s="23">
+        <v>32</v>
+      </c>
+      <c r="S6" s="24">
         <v>500</v>
       </c>
-      <c r="T6" s="25">
+      <c r="U6" s="26">
         <v>45846</v>
       </c>
-      <c r="U6" s="26">
-        <v>.2916666666666673352208</v>
-      </c>
       <c r="V6" s="27">
-        <v>0</v>
+        <v>.5000000000000011460928</v>
       </c>
       <c r="W6" s="28">
+        <v>0</v>
+      </c>
+      <c r="X6" s="29">
         <v>15</v>
       </c>
-      <c r="X6" s="29">
+      <c r="Y6" s="30">
         <v>2</v>
       </c>
-      <c r="Y6" s="30">
-        <v>5</v>
-      </c>
       <c r="Z6" s="31">
+        <v>5</v>
+      </c>
+      <c r="AA6" s="32">
         <v>10</v>
       </c>
-      <c r="AA6" s="32">
+      <c r="AB6" s="33">
         <v>.5</v>
       </c>
-      <c r="AB6" s="33">
+      <c r="AC6" s="34">
         <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="6">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B7" s="7">
         <v>0</v>
@@ -862,56 +877,56 @@
         <v>120</v>
       </c>
       <c r="E7" t="s" s="10">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F7" s="11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G7" s="12">
         <v>70</v>
       </c>
       <c r="H7" s="13">
+        <v>280</v>
+      </c>
+      <c r="I7" s="14">
         <v>20</v>
       </c>
-      <c r="I7" s="14">
+      <c r="J7" s="15">
         <v>6</v>
       </c>
-      <c r="J7" s="15">
+      <c r="K7" s="16">
         <v>1050</v>
       </c>
-      <c r="K7" t="s" s="16">
-        <v>42</v>
-      </c>
-      <c r="L7" s="17">
+      <c r="L7" t="s" s="17">
+        <v>43</v>
+      </c>
+      <c r="M7" s="18">
         <v>750</v>
       </c>
-      <c r="O7" s="20">
+      <c r="P7" s="21">
         <v>8</v>
       </c>
-      <c r="P7" s="21">
+      <c r="Q7" s="22">
         <v>1050</v>
       </c>
-      <c r="Q7" t="s" s="22">
-        <v>31</v>
-      </c>
-      <c r="R7" s="23">
+      <c r="R7" t="s" s="23">
+        <v>32</v>
+      </c>
+      <c r="S7" s="24">
         <v>420</v>
       </c>
-      <c r="T7" s="25">
+      <c r="U7" s="26">
         <v>45846</v>
       </c>
-      <c r="U7" s="26">
-        <v>.2916666666666673352208</v>
-      </c>
       <c r="V7" s="27">
+        <v>.5000000000000011460928</v>
+      </c>
+      <c r="W7" s="28">
         <v>2</v>
       </c>
-      <c r="W7" s="28">
+      <c r="X7" s="29">
         <v>15</v>
       </c>
-      <c r="X7" s="29">
-        <v>5</v>
-      </c>
       <c r="Y7" s="30">
         <v>5</v>
       </c>
@@ -922,12 +937,15 @@
         <v>5</v>
       </c>
       <c r="AB7" s="33">
+        <v>5</v>
+      </c>
+      <c r="AC7" s="34">
         <v>5</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="6">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B8" s="7">
         <v>1</v>
@@ -939,72 +957,78 @@
         <v>120</v>
       </c>
       <c r="E8" t="s" s="10">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F8" s="11">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="G8" s="12">
+        <v>76</v>
       </c>
       <c r="H8" s="13">
         <v>400</v>
       </c>
       <c r="I8" s="14">
+        <v>400</v>
+      </c>
+      <c r="J8" s="15">
         <v>7</v>
       </c>
-      <c r="J8" s="15">
+      <c r="K8" s="16">
         <v>1350</v>
       </c>
-      <c r="K8" t="s" s="16">
-        <v>44</v>
-      </c>
-      <c r="L8" s="17">
+      <c r="L8" t="s" s="17">
+        <v>45</v>
+      </c>
+      <c r="M8" s="18">
         <v>800</v>
       </c>
-      <c r="O8" s="20">
+      <c r="P8" s="21">
         <v>10</v>
       </c>
-      <c r="P8" s="21">
+      <c r="Q8" s="22">
         <v>1000</v>
       </c>
-      <c r="Q8" t="s" s="22">
-        <v>31</v>
-      </c>
-      <c r="R8" s="23">
+      <c r="R8" t="s" s="23">
+        <v>32</v>
+      </c>
+      <c r="S8" s="24">
         <v>500</v>
       </c>
-      <c r="S8" s="24">
+      <c r="T8" s="25">
         <v>50</v>
       </c>
-      <c r="T8" s="25">
+      <c r="U8" s="26">
         <v>45846</v>
       </c>
-      <c r="U8" s="26">
-        <v>.2916666666666673352208</v>
-      </c>
       <c r="V8" s="27">
-        <v>15</v>
+        <v>.5000000000000011460928</v>
       </c>
       <c r="W8" s="28">
         <v>15</v>
       </c>
       <c r="X8" s="29">
+        <v>15</v>
+      </c>
+      <c r="Y8" s="30">
         <v>2</v>
       </c>
-      <c r="Y8" s="30">
-        <v>5</v>
-      </c>
       <c r="Z8" s="31">
         <v>5</v>
       </c>
       <c r="AA8" s="32">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AB8" s="33">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="34">
         <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="6">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B9" s="7">
         <v>1</v>
@@ -1016,56 +1040,53 @@
         <v>120</v>
       </c>
       <c r="E9" t="s" s="10">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F9" s="11">
-        <v>1</v>
-      </c>
-      <c r="G9" s="12">
-        <v>70</v>
+        <v>3</v>
       </c>
       <c r="H9" s="13">
-        <v>0</v>
+        <v>286</v>
       </c>
       <c r="I9" s="14">
+        <v>0</v>
+      </c>
+      <c r="J9" s="15">
         <v>8</v>
       </c>
-      <c r="J9" s="15">
+      <c r="K9" s="16">
         <v>1300</v>
       </c>
-      <c r="K9" t="s" s="16">
-        <v>46</v>
-      </c>
-      <c r="L9" s="17">
+      <c r="L9" t="s" s="17">
+        <v>47</v>
+      </c>
+      <c r="M9" s="18">
         <v>1000</v>
       </c>
-      <c r="O9" s="20">
+      <c r="P9" s="21">
         <v>10</v>
       </c>
-      <c r="P9" s="21">
+      <c r="Q9" s="22">
         <v>1260</v>
       </c>
-      <c r="Q9" t="s" s="22">
-        <v>34</v>
-      </c>
-      <c r="R9" s="23">
+      <c r="R9" t="s" s="23">
+        <v>35</v>
+      </c>
+      <c r="S9" s="24">
         <v>600</v>
       </c>
-      <c r="T9" s="25">
+      <c r="U9" s="26">
         <v>45846</v>
       </c>
-      <c r="U9" s="26">
-        <v>.2916666666666673352208</v>
-      </c>
       <c r="V9" s="27">
-        <v>5</v>
+        <v>.5000000000000011460928</v>
       </c>
       <c r="W9" s="28">
+        <v>5</v>
+      </c>
+      <c r="X9" s="29">
         <v>10</v>
       </c>
-      <c r="X9" s="29">
-        <v>5</v>
-      </c>
       <c r="Y9" s="30">
         <v>5</v>
       </c>
@@ -1076,12 +1097,15 @@
         <v>5</v>
       </c>
       <c r="AB9" s="33">
+        <v>5</v>
+      </c>
+      <c r="AC9" s="34">
         <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="6">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B10" s="7">
         <v>0</v>
@@ -1093,59 +1117,50 @@
         <v>120</v>
       </c>
       <c r="E10" t="s" s="10">
-        <v>29</v>
-      </c>
-      <c r="F10" s="11">
-        <v>4</v>
-      </c>
-      <c r="G10" s="12">
-        <v>70</v>
-      </c>
-      <c r="H10" s="13">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="I10" s="14">
+        <v>0</v>
+      </c>
+      <c r="J10" s="15">
         <v>9</v>
       </c>
-      <c r="J10" s="15">
+      <c r="K10" s="16">
         <v>910</v>
       </c>
-      <c r="K10" t="s" s="16">
-        <v>48</v>
-      </c>
-      <c r="L10" s="17">
+      <c r="L10" t="s" s="17">
+        <v>49</v>
+      </c>
+      <c r="M10" s="18">
         <v>620</v>
       </c>
-      <c r="O10" s="20">
+      <c r="P10" s="21">
         <v>37</v>
       </c>
-      <c r="P10" s="21">
+      <c r="Q10" s="22">
         <v>900</v>
       </c>
-      <c r="Q10" t="s" s="22">
-        <v>34</v>
-      </c>
-      <c r="R10" s="23">
+      <c r="R10" t="s" s="23">
+        <v>35</v>
+      </c>
+      <c r="S10" s="24">
         <v>450</v>
       </c>
-      <c r="S10" s="24">
+      <c r="T10" s="25">
         <v>18</v>
       </c>
-      <c r="T10" s="25">
+      <c r="U10" s="26">
         <v>45846</v>
       </c>
-      <c r="U10" s="26">
-        <v>.2916666666666673352208</v>
-      </c>
       <c r="V10" s="27">
+        <v>.5000000000000011460928</v>
+      </c>
+      <c r="W10" s="28">
         <v>2</v>
       </c>
-      <c r="W10" s="28">
+      <c r="X10" s="29">
         <v>15</v>
       </c>
-      <c r="X10" s="29">
-        <v>5</v>
-      </c>
       <c r="Y10" s="30">
         <v>5</v>
       </c>
@@ -1156,12 +1171,15 @@
         <v>5</v>
       </c>
       <c r="AB10" s="33">
+        <v>5</v>
+      </c>
+      <c r="AC10" s="34">
         <v>5</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="6">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B11" s="7">
         <v>1</v>
@@ -1173,58 +1191,58 @@
         <v>120</v>
       </c>
       <c r="E11" t="s" s="10">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F11" s="11">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="G11" s="12">
         <v>70</v>
       </c>
       <c r="H11" s="13">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="I11" s="14">
+        <v>0</v>
+      </c>
+      <c r="J11" s="15">
         <v>10</v>
       </c>
-      <c r="J11" s="15">
+      <c r="K11" s="16">
         <v>1080</v>
       </c>
-      <c r="K11" t="s" s="16">
-        <v>50</v>
-      </c>
-      <c r="L11" s="17">
+      <c r="L11" t="s" s="17">
+        <v>51</v>
+      </c>
+      <c r="M11" s="18">
         <v>800</v>
       </c>
-      <c r="O11" s="20">
+      <c r="P11" s="21">
         <v>24</v>
       </c>
-      <c r="P11" s="21">
+      <c r="Q11" s="22">
         <v>530</v>
       </c>
-      <c r="Q11" t="s" s="22">
-        <v>31</v>
-      </c>
-      <c r="R11" s="23">
+      <c r="R11" t="s" s="23">
+        <v>32</v>
+      </c>
+      <c r="S11" s="24">
         <v>600</v>
       </c>
-      <c r="S11" s="24">
+      <c r="T11" s="25">
         <v>40</v>
       </c>
-      <c r="T11" s="25">
+      <c r="U11" s="26">
         <v>45846</v>
       </c>
-      <c r="U11" s="26">
-        <v>.2916666666666673352208</v>
-      </c>
       <c r="V11" s="27">
-        <v>10</v>
+        <v>.5000000000000011460928</v>
       </c>
       <c r="W11" s="28">
         <v>10</v>
       </c>
       <c r="X11" s="29">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="Y11" s="30">
         <v>5</v>
@@ -1236,12 +1254,15 @@
         <v>5</v>
       </c>
       <c r="AB11" s="33">
+        <v>5</v>
+      </c>
+      <c r="AC11" s="34">
         <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="6">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B12" s="7">
         <v>1</v>
@@ -1253,7 +1274,7 @@
         <v>120</v>
       </c>
       <c r="E12" t="s" s="10">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F12" s="11">
         <v>3</v>
@@ -1262,47 +1283,47 @@
         <v>152</v>
       </c>
       <c r="H12" s="13">
-        <v>0</v>
+        <v>408</v>
       </c>
       <c r="I12" s="14">
+        <v>0</v>
+      </c>
+      <c r="J12" s="15">
         <v>11</v>
       </c>
-      <c r="J12" s="15">
+      <c r="K12" s="16">
         <v>1300</v>
       </c>
-      <c r="K12" t="s" s="16">
-        <v>52</v>
-      </c>
-      <c r="L12" s="17">
+      <c r="L12" t="s" s="17">
+        <v>53</v>
+      </c>
+      <c r="M12" s="18">
         <v>1000</v>
       </c>
-      <c r="O12" s="20">
+      <c r="P12" s="21">
         <v>10</v>
       </c>
-      <c r="P12" s="21">
+      <c r="Q12" s="22">
         <v>1260</v>
       </c>
-      <c r="Q12" t="s" s="22">
-        <v>34</v>
-      </c>
-      <c r="R12" s="23">
+      <c r="R12" t="s" s="23">
+        <v>35</v>
+      </c>
+      <c r="S12" s="24">
         <v>600</v>
       </c>
-      <c r="T12" s="25">
+      <c r="U12" s="26">
         <v>45846</v>
       </c>
-      <c r="U12" s="26">
-        <v>.2916666666666673352208</v>
-      </c>
       <c r="V12" s="27">
-        <v>5</v>
+        <v>.5000000000000011460928</v>
       </c>
       <c r="W12" s="28">
+        <v>5</v>
+      </c>
+      <c r="X12" s="29">
         <v>10</v>
       </c>
-      <c r="X12" s="29">
-        <v>5</v>
-      </c>
       <c r="Y12" s="30">
         <v>5</v>
       </c>
@@ -1313,12 +1334,15 @@
         <v>5</v>
       </c>
       <c r="AB12" s="33">
+        <v>5</v>
+      </c>
+      <c r="AC12" s="34">
         <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="6">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B13" s="7">
         <v>1</v>
@@ -1330,7 +1354,7 @@
         <v>120</v>
       </c>
       <c r="E13" t="s" s="10">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F13" s="11">
         <v>2</v>
@@ -1339,66 +1363,69 @@
         <v>76</v>
       </c>
       <c r="H13" s="13">
+        <v>480</v>
+      </c>
+      <c r="I13" s="14">
         <v>400</v>
       </c>
-      <c r="I13" s="14">
+      <c r="J13" s="15">
         <v>12</v>
       </c>
-      <c r="J13" s="15">
+      <c r="K13" s="16">
         <v>1350</v>
       </c>
-      <c r="K13" t="s" s="16">
-        <v>54</v>
-      </c>
-      <c r="L13" s="17">
+      <c r="L13" t="s" s="17">
+        <v>55</v>
+      </c>
+      <c r="M13" s="18">
         <v>800</v>
       </c>
-      <c r="O13" s="20">
+      <c r="P13" s="21">
         <v>10</v>
       </c>
-      <c r="P13" s="21">
+      <c r="Q13" s="22">
         <v>1000</v>
       </c>
-      <c r="Q13" t="s" s="22">
-        <v>34</v>
-      </c>
-      <c r="R13" s="23">
+      <c r="R13" t="s" s="23">
+        <v>35</v>
+      </c>
+      <c r="S13" s="24">
         <v>500</v>
       </c>
-      <c r="S13" s="24">
+      <c r="T13" s="25">
         <v>50</v>
       </c>
-      <c r="T13" s="25">
+      <c r="U13" s="26">
         <v>45846</v>
       </c>
-      <c r="U13" s="26">
-        <v>.2916666666666673352208</v>
-      </c>
       <c r="V13" s="27">
+        <v>.5000000000000011460928</v>
+      </c>
+      <c r="W13" s="28">
         <v>15</v>
       </c>
-      <c r="W13" s="28">
-        <v>5</v>
-      </c>
       <c r="X13" s="29">
+        <v>5</v>
+      </c>
+      <c r="Y13" s="30">
         <v>2</v>
       </c>
-      <c r="Y13" s="30">
-        <v>5</v>
-      </c>
       <c r="Z13" s="31">
         <v>5</v>
       </c>
       <c r="AA13" s="32">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AB13" s="33">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="34">
         <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="6">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B14" s="7">
         <v>0</v>
@@ -1410,42 +1437,42 @@
         <v>120</v>
       </c>
       <c r="E14" t="s" s="10">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F14" t="s" s="11">
-        <v>57</v>
-      </c>
-      <c r="H14" s="13">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="I14" s="14">
+        <v>0</v>
+      </c>
+      <c r="J14" s="15">
         <v>13</v>
       </c>
-      <c r="J14" s="15">
+      <c r="K14" s="16">
         <v>810</v>
       </c>
-      <c r="K14" t="s" s="16">
-        <v>58</v>
-      </c>
-      <c r="L14" s="17">
+      <c r="L14" t="s" s="17">
+        <v>59</v>
+      </c>
+      <c r="M14" s="18">
         <v>800</v>
       </c>
-      <c r="M14" s="18">
+      <c r="N14" s="19">
         <v>330</v>
       </c>
-      <c r="N14" s="19">
+      <c r="O14" s="20">
         <v>640</v>
       </c>
-      <c r="T14" s="25">
+      <c r="U14" s="26">
         <v>45846</v>
       </c>
-      <c r="U14" s="26">
-        <v>.2916666666666673352208</v>
+      <c r="V14" s="27">
+        <v>.5000000000000011460928</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="6">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B15" s="7">
         <v>0</v>
@@ -1457,42 +1484,39 @@
         <v>120</v>
       </c>
       <c r="E15" t="s" s="10">
-        <v>56</v>
-      </c>
-      <c r="F15" t="s" s="11">
         <v>57</v>
       </c>
-      <c r="H15" s="13">
-        <v>0</v>
-      </c>
       <c r="I15" s="14">
+        <v>0</v>
+      </c>
+      <c r="J15" s="15">
         <v>14</v>
       </c>
-      <c r="J15" s="15">
+      <c r="K15" s="16">
         <v>1050</v>
       </c>
-      <c r="K15" t="s" s="16">
-        <v>60</v>
-      </c>
-      <c r="L15" s="17">
+      <c r="L15" t="s" s="17">
+        <v>61</v>
+      </c>
+      <c r="M15" s="18">
         <v>800</v>
       </c>
-      <c r="M15" s="18">
+      <c r="N15" s="19">
         <v>400</v>
       </c>
-      <c r="N15" s="19">
+      <c r="O15" s="20">
         <v>1000</v>
       </c>
-      <c r="T15" s="25">
+      <c r="U15" s="26">
         <v>45846</v>
       </c>
-      <c r="U15" s="26">
-        <v>.2916666666666673352208</v>
+      <c r="V15" s="27">
+        <v>.5000000000000011460928</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="6">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B16" s="7">
         <v>0</v>
@@ -1504,42 +1528,42 @@
         <v>120</v>
       </c>
       <c r="E16" t="s" s="10">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F16" t="s" s="11">
-        <v>57</v>
-      </c>
-      <c r="H16" s="13">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="I16" s="14">
+        <v>0</v>
+      </c>
+      <c r="J16" s="15">
         <v>15</v>
       </c>
-      <c r="J16" s="15">
+      <c r="K16" s="16">
         <v>910</v>
       </c>
-      <c r="K16" t="s" s="16">
-        <v>62</v>
-      </c>
-      <c r="L16" s="17">
+      <c r="L16" t="s" s="17">
+        <v>63</v>
+      </c>
+      <c r="M16" s="18">
         <v>800</v>
       </c>
-      <c r="M16" s="18">
+      <c r="N16" s="19">
         <v>300</v>
       </c>
-      <c r="N16" s="19">
+      <c r="O16" s="20">
         <v>1150</v>
       </c>
-      <c r="T16" s="25">
+      <c r="U16" s="26">
         <v>45846</v>
       </c>
-      <c r="U16" s="26">
-        <v>.2916666666666673352208</v>
+      <c r="V16" s="27">
+        <v>.5000000000000011460928</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="6">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B17" s="7">
         <v>0</v>
@@ -1551,42 +1575,39 @@
         <v>120</v>
       </c>
       <c r="E17" t="s" s="10">
-        <v>56</v>
-      </c>
-      <c r="F17" t="s" s="11">
         <v>57</v>
       </c>
-      <c r="H17" s="13">
-        <v>0</v>
-      </c>
       <c r="I17" s="14">
+        <v>0</v>
+      </c>
+      <c r="J17" s="15">
         <v>16</v>
       </c>
-      <c r="J17" s="15">
+      <c r="K17" s="16">
         <v>1220</v>
       </c>
-      <c r="K17" t="s" s="16">
-        <v>64</v>
-      </c>
-      <c r="L17" s="17">
+      <c r="L17" t="s" s="17">
+        <v>65</v>
+      </c>
+      <c r="M17" s="18">
         <v>800</v>
       </c>
-      <c r="M17" s="18">
+      <c r="N17" s="19">
         <v>400</v>
       </c>
-      <c r="N17" s="19">
+      <c r="O17" s="20">
         <v>1500</v>
       </c>
-      <c r="T17" s="25">
+      <c r="U17" s="26">
         <v>45846</v>
       </c>
-      <c r="U17" s="26">
-        <v>.2916666666666673352208</v>
+      <c r="V17" s="27">
+        <v>.5000000000000011460928</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="6">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B18" s="7">
         <v>0</v>
@@ -1598,37 +1619,37 @@
         <v>120</v>
       </c>
       <c r="E18" t="s" s="10">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F18" t="s" s="11">
-        <v>57</v>
-      </c>
-      <c r="H18" s="13">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="I18" s="14">
+        <v>0</v>
+      </c>
+      <c r="J18" s="15">
         <v>17</v>
       </c>
-      <c r="J18" s="15">
+      <c r="K18" s="16">
         <v>1050</v>
       </c>
-      <c r="K18" t="s" s="16">
-        <v>66</v>
-      </c>
-      <c r="L18" s="17">
+      <c r="L18" t="s" s="17">
+        <v>67</v>
+      </c>
+      <c r="M18" s="18">
         <v>800</v>
       </c>
-      <c r="M18" s="18">
+      <c r="N18" s="19">
         <v>400</v>
       </c>
-      <c r="N18" s="19">
+      <c r="O18" s="20">
         <v>1000</v>
       </c>
-      <c r="T18" s="25">
+      <c r="U18" s="26">
         <v>45846</v>
       </c>
-      <c r="U18" s="26">
-        <v>.2916666666666673352208</v>
+      <c r="V18" s="27">
+        <v>.5000000000000011460928</v>
       </c>
     </row>
   </sheetData>

</xml_diff>